<commit_message>
Modified data models. Added Email class
</commit_message>
<xml_diff>
--- a/project notes/database schema.xlsx
+++ b/project notes/database schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="10480" yWindow="0" windowWidth="17280" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>Referral puppy</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Database Schema</t>
   </si>
   <si>
-    <t>USER TABLE</t>
-  </si>
-  <si>
     <t>first</t>
   </si>
   <si>
@@ -39,12 +36,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>passwordhash+salt</t>
-  </si>
-  <si>
-    <t>group id</t>
-  </si>
-  <si>
     <t>REFERRAL TABLE</t>
   </si>
   <si>
@@ -63,52 +54,184 @@
     <t>date</t>
   </si>
   <si>
-    <t>date_created</t>
+    <t>note_from_giver</t>
+  </si>
+  <si>
+    <t>dave</t>
+  </si>
+  <si>
+    <t>stewart</t>
+  </si>
+  <si>
+    <t>davestewart@gmail.com</t>
+  </si>
+  <si>
+    <t>djsdgsadgs29239sdjh</t>
+  </si>
+  <si>
+    <t>15-4-2014</t>
+  </si>
+  <si>
+    <t>business_referred</t>
+  </si>
+  <si>
+    <t>gilman and associated, lawyers</t>
+  </si>
+  <si>
+    <t>law firm looking for headshots</t>
+  </si>
+  <si>
+    <t>karen</t>
+  </si>
+  <si>
+    <t>alvarez</t>
+  </si>
+  <si>
+    <t>skdjhs@hotmail.com</t>
+  </si>
+  <si>
+    <t>sakjfhsdkjfhdsfjh</t>
+  </si>
+  <si>
+    <t>attorney</t>
+  </si>
+  <si>
+    <t>photographer</t>
+  </si>
+  <si>
+    <t>authenticated?</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>USER TABLE (django built in)</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>ENTITIES and ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>address 1</t>
+  </si>
+  <si>
+    <t>address 2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>referrals given</t>
+  </si>
+  <si>
+    <t>referrals received</t>
+  </si>
+  <si>
+    <t>joined</t>
   </si>
   <si>
     <t>last_login</t>
   </si>
   <si>
-    <t>note_from_giver</t>
-  </si>
-  <si>
-    <t>dave</t>
-  </si>
-  <si>
-    <t>stewart</t>
-  </si>
-  <si>
-    <t>davestewart@gmail.com</t>
-  </si>
-  <si>
-    <t>djsdgsadgs29239sdjh</t>
-  </si>
-  <si>
-    <t>15-4-2014</t>
-  </si>
-  <si>
-    <t>business_referred</t>
-  </si>
-  <si>
-    <t>gilman and associated, lawyers</t>
-  </si>
-  <si>
-    <t>law firm looking for headshots</t>
-  </si>
-  <si>
-    <t>karen</t>
-  </si>
-  <si>
-    <t>alvarez</t>
-  </si>
-  <si>
-    <t>skdjhs@hotmail.com</t>
-  </si>
-  <si>
-    <t>sakjfhsdkjfhdsfjh</t>
-  </si>
-  <si>
-    <t>profession</t>
+    <t>referrer score</t>
+  </si>
+  <si>
+    <t>referee score</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>blog</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>created date</t>
+  </si>
+  <si>
+    <t>modified date</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>approved (y/n)</t>
+  </si>
+  <si>
+    <t>credit card #</t>
+  </si>
+  <si>
+    <t>CC exp date</t>
+  </si>
+  <si>
+    <t>userID (PK)</t>
+  </si>
+  <si>
+    <t>referenceID(PK)</t>
+  </si>
+  <si>
+    <t>blogPostID (PK)</t>
+  </si>
+  <si>
+    <t>commentID (PK)</t>
+  </si>
+  <si>
+    <t>commentText</t>
+  </si>
+  <si>
+    <t>author (FK - user)</t>
+  </si>
+  <si>
+    <t>blogPostID (FK - blog)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biz/person referred (FK - user) </t>
+  </si>
+  <si>
+    <t>receiver (FK - user)</t>
+  </si>
+  <si>
+    <t>giver (FK - user)</t>
+  </si>
+  <si>
+    <t>cashValue (segun giver)</t>
+  </si>
+  <si>
+    <t>cashValue (segun receiver)</t>
   </si>
 </sst>
 </file>
@@ -170,10 +293,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -507,16 +631,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I24"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
     <col min="3" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="41.83203125" customWidth="1"/>
@@ -525,116 +649,110 @@
     <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:6">
       <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>1</v>
       </c>
@@ -645,13 +763,197 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +962,6 @@
     <hyperlink ref="E11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>